<commit_message>
Update examples for improv test.xlsx
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/examples for improv test.xlsx
+++ b/migforecasting/clustering/examples for improv test.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="examples" sheetId="1" r:id="rId1"/>
+    <sheet name="examples abs (for model)" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
   <si>
     <t>oktmo</t>
   </si>
@@ -178,7 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +191,15 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -305,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -335,6 +345,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -619,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2653,4 +2669,2041 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="37.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="20" max="21" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>22719000</v>
+      </c>
+      <c r="B2" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11">
+        <v>-140</v>
+      </c>
+      <c r="F2" s="11">
+        <v>17275</v>
+      </c>
+      <c r="G2" s="11">
+        <v>2414</v>
+      </c>
+      <c r="H2" s="11">
+        <v>19887.443500000001</v>
+      </c>
+      <c r="I2" s="11">
+        <v>8104.9999999999982</v>
+      </c>
+      <c r="J2" s="11">
+        <v>473.99999999999983</v>
+      </c>
+      <c r="K2" s="11">
+        <v>729883.93608999986</v>
+      </c>
+      <c r="L2" s="11">
+        <v>39.4</v>
+      </c>
+      <c r="M2" s="11">
+        <v>44.999999999999716</v>
+      </c>
+      <c r="N2" s="11">
+        <v>7.99999999999996</v>
+      </c>
+      <c r="O2" s="11">
+        <v>296.89999999999964</v>
+      </c>
+      <c r="P2" s="11">
+        <v>32143.999999999978</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>60102.41</v>
+      </c>
+      <c r="R2" s="11">
+        <v>550648.19779999938</v>
+      </c>
+      <c r="S2" s="11">
+        <v>22.999999999999957</v>
+      </c>
+      <c r="T2" s="11">
+        <v>946</v>
+      </c>
+      <c r="U2" s="11">
+        <v>236233.5437799996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>3639000</v>
+      </c>
+      <c r="B3" s="11">
+        <v>2019</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11">
+        <v>-476</v>
+      </c>
+      <c r="F3" s="11">
+        <v>65842</v>
+      </c>
+      <c r="G3" s="11">
+        <v>10892</v>
+      </c>
+      <c r="H3" s="11">
+        <v>21988.19528</v>
+      </c>
+      <c r="I3" s="11">
+        <v>37427.899999999994</v>
+      </c>
+      <c r="J3" s="11">
+        <v>807.99999999999966</v>
+      </c>
+      <c r="K3" s="11">
+        <v>2824760.7281099996</v>
+      </c>
+      <c r="L3" s="11">
+        <v>25</v>
+      </c>
+      <c r="M3" s="11">
+        <v>78.999999999999503</v>
+      </c>
+      <c r="N3" s="11">
+        <v>242.99999999999901</v>
+      </c>
+      <c r="O3" s="11">
+        <v>632.49999999999932</v>
+      </c>
+      <c r="P3" s="11">
+        <v>959880.00000000023</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>322825.61999999994</v>
+      </c>
+      <c r="R3" s="11">
+        <v>12665201.631199995</v>
+      </c>
+      <c r="S3" s="11">
+        <v>25.999999999999947</v>
+      </c>
+      <c r="T3" s="11">
+        <v>3185</v>
+      </c>
+      <c r="U3" s="11">
+        <v>12405299.012639996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>3657000</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>-898</v>
+      </c>
+      <c r="F4" s="11">
+        <v>110482</v>
+      </c>
+      <c r="G4" s="11">
+        <v>18706.999999999996</v>
+      </c>
+      <c r="H4" s="11">
+        <v>21442.174780000001</v>
+      </c>
+      <c r="I4" s="11">
+        <v>71187.999999999971</v>
+      </c>
+      <c r="J4" s="11">
+        <v>3068.9999999999986</v>
+      </c>
+      <c r="K4" s="11">
+        <v>1434081.5877000005</v>
+      </c>
+      <c r="L4" s="11">
+        <v>24.9</v>
+      </c>
+      <c r="M4" s="11">
+        <v>208.99999999999864</v>
+      </c>
+      <c r="N4" s="11">
+        <v>249.99999999999895</v>
+      </c>
+      <c r="O4" s="11">
+        <v>760.29999999999905</v>
+      </c>
+      <c r="P4" s="11">
+        <v>82717.999999999985</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>330035.92</v>
+      </c>
+      <c r="R4" s="11">
+        <v>11480639.036999995</v>
+      </c>
+      <c r="S4" s="11">
+        <v>29.999999999999915</v>
+      </c>
+      <c r="T4" s="11">
+        <v>4768.9999999999991</v>
+      </c>
+      <c r="U4" s="11">
+        <v>15406913.946689995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>14625000</v>
+      </c>
+      <c r="B5" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11">
+        <v>-166</v>
+      </c>
+      <c r="F5" s="11">
+        <v>18562</v>
+      </c>
+      <c r="G5" s="11">
+        <v>3694.0000000000009</v>
+      </c>
+      <c r="H5" s="11">
+        <v>21712.38264</v>
+      </c>
+      <c r="I5" s="11">
+        <v>8165.7999999999993</v>
+      </c>
+      <c r="J5" s="11">
+        <v>567.99999999999966</v>
+      </c>
+      <c r="K5" s="11">
+        <v>479171.98727999994</v>
+      </c>
+      <c r="L5" s="11">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="M5" s="11">
+        <v>94.999999999999403</v>
+      </c>
+      <c r="N5" s="11">
+        <v>41.999999999999844</v>
+      </c>
+      <c r="O5" s="11">
+        <v>556.39999999999964</v>
+      </c>
+      <c r="P5" s="11">
+        <v>14808.999999999978</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>36416.79</v>
+      </c>
+      <c r="R5" s="11">
+        <v>4968189.5378400004</v>
+      </c>
+      <c r="S5" s="11">
+        <v>23.99999999999994</v>
+      </c>
+      <c r="T5" s="11">
+        <v>958.99999999999977</v>
+      </c>
+      <c r="U5" s="11">
+        <v>1727129.7467999991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>18610000</v>
+      </c>
+      <c r="B6" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11">
+        <v>-210</v>
+      </c>
+      <c r="F6" s="11">
+        <v>28673</v>
+      </c>
+      <c r="G6" s="11">
+        <v>4213</v>
+      </c>
+      <c r="H6" s="11">
+        <v>18718.034879999999</v>
+      </c>
+      <c r="I6" s="11">
+        <v>15706.399999999994</v>
+      </c>
+      <c r="J6" s="11">
+        <v>1185.9999999999993</v>
+      </c>
+      <c r="K6" s="11">
+        <v>912846.19063000008</v>
+      </c>
+      <c r="L6" s="11">
+        <v>36.5</v>
+      </c>
+      <c r="M6" s="11">
+        <v>107.99999999999929</v>
+      </c>
+      <c r="N6" s="11">
+        <v>91.999999999999645</v>
+      </c>
+      <c r="O6" s="11">
+        <v>873.59999999999934</v>
+      </c>
+      <c r="P6" s="11">
+        <v>127582.99999999996</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>56902.999999999993</v>
+      </c>
+      <c r="R6" s="11">
+        <v>5517088.4192999983</v>
+      </c>
+      <c r="S6" s="11">
+        <v>38.999999999999915</v>
+      </c>
+      <c r="T6" s="11">
+        <v>1113.0000000000002</v>
+      </c>
+      <c r="U6" s="11">
+        <v>6142682.3205399979</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>1703000</v>
+      </c>
+      <c r="B7" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11">
+        <v>-291</v>
+      </c>
+      <c r="F7" s="11">
+        <v>28434</v>
+      </c>
+      <c r="G7" s="11">
+        <v>5725</v>
+      </c>
+      <c r="H7" s="11">
+        <v>20773.66617</v>
+      </c>
+      <c r="I7" s="11">
+        <v>26868.199999999993</v>
+      </c>
+      <c r="J7" s="11">
+        <v>1111.9999999999993</v>
+      </c>
+      <c r="K7" s="11">
+        <v>1674021.9106300003</v>
+      </c>
+      <c r="L7" s="11">
+        <v>22.6</v>
+      </c>
+      <c r="M7" s="11">
+        <v>72.999999999999545</v>
+      </c>
+      <c r="N7" s="11">
+        <v>113.99999999999952</v>
+      </c>
+      <c r="O7" s="11">
+        <v>350.99999999999966</v>
+      </c>
+      <c r="P7" s="11">
+        <v>10711.999999999955</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>7011.1399999999894</v>
+      </c>
+      <c r="R7" s="11">
+        <v>49916.868199999284</v>
+      </c>
+      <c r="S7" s="11">
+        <v>1.9999999999999927</v>
+      </c>
+      <c r="T7" s="11">
+        <v>1617.9999999999998</v>
+      </c>
+      <c r="U7" s="11">
+        <v>5355232.274249997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>1716000</v>
+      </c>
+      <c r="B8" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11">
+        <v>-284</v>
+      </c>
+      <c r="F8" s="11">
+        <v>139565</v>
+      </c>
+      <c r="G8" s="11">
+        <v>24379.999999999993</v>
+      </c>
+      <c r="H8" s="11">
+        <v>19874.44096</v>
+      </c>
+      <c r="I8" s="11">
+        <v>207240.69999999998</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1859.9999999999984</v>
+      </c>
+      <c r="K8" s="11">
+        <v>5926777.3109299988</v>
+      </c>
+      <c r="L8" s="11">
+        <v>21.6</v>
+      </c>
+      <c r="M8" s="11">
+        <v>311.9999999999979</v>
+      </c>
+      <c r="N8" s="11">
+        <v>386.99999999999841</v>
+      </c>
+      <c r="O8" s="11">
+        <v>962.79999999999893</v>
+      </c>
+      <c r="P8" s="11">
+        <v>8125.9999999999918</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>44861.889999999948</v>
+      </c>
+      <c r="R8" s="11">
+        <v>199155.57099999874</v>
+      </c>
+      <c r="S8" s="11">
+        <v>33.999999999999922</v>
+      </c>
+      <c r="T8" s="11">
+        <v>6249</v>
+      </c>
+      <c r="U8" s="11">
+        <v>15178335.903369986</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>10615000</v>
+      </c>
+      <c r="B9" s="11">
+        <v>2019</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11">
+        <v>-274</v>
+      </c>
+      <c r="F9" s="11">
+        <v>19887.999999999989</v>
+      </c>
+      <c r="G9" s="11">
+        <v>4481.9999999999982</v>
+      </c>
+      <c r="H9" s="11">
+        <v>37917.462079999998</v>
+      </c>
+      <c r="I9" s="11">
+        <v>14558.999999999989</v>
+      </c>
+      <c r="J9" s="11">
+        <v>609.99999999999943</v>
+      </c>
+      <c r="K9" s="11">
+        <v>1282627.8831299993</v>
+      </c>
+      <c r="L9" s="11">
+        <v>29.1</v>
+      </c>
+      <c r="M9" s="11">
+        <v>67.999999999999545</v>
+      </c>
+      <c r="N9" s="11">
+        <v>114.99999999999949</v>
+      </c>
+      <c r="O9" s="11">
+        <v>358.69999999999959</v>
+      </c>
+      <c r="P9" s="11">
+        <v>4886.9999999999818</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>8000.4999999999918</v>
+      </c>
+      <c r="R9" s="11">
+        <v>794969.88139999914</v>
+      </c>
+      <c r="S9" s="11">
+        <v>14.999999999999956</v>
+      </c>
+      <c r="T9" s="11">
+        <v>1094.9999999999995</v>
+      </c>
+      <c r="U9" s="11">
+        <v>5006117.3553799978</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>10710000</v>
+      </c>
+      <c r="B10" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="11">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11">
+        <v>-340</v>
+      </c>
+      <c r="F10" s="11">
+        <v>65776</v>
+      </c>
+      <c r="G10" s="11">
+        <v>14881</v>
+      </c>
+      <c r="H10" s="11">
+        <v>35840.741759999997</v>
+      </c>
+      <c r="I10" s="11">
+        <v>52247.999999999993</v>
+      </c>
+      <c r="J10" s="11">
+        <v>2190.9999999999991</v>
+      </c>
+      <c r="K10" s="11">
+        <v>2740590.23832</v>
+      </c>
+      <c r="L10" s="11">
+        <v>22.8</v>
+      </c>
+      <c r="M10" s="11">
+        <v>240.99999999999852</v>
+      </c>
+      <c r="N10" s="11">
+        <v>194.99999999999918</v>
+      </c>
+      <c r="O10" s="11">
+        <v>225.39999999999938</v>
+      </c>
+      <c r="P10" s="11">
+        <v>2243.9999999999036</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>11420.029999999982</v>
+      </c>
+      <c r="R10" s="11">
+        <v>169468.43350463765</v>
+      </c>
+      <c r="S10" s="11">
+        <v>5.9999999999999716</v>
+      </c>
+      <c r="T10" s="11">
+        <v>3302</v>
+      </c>
+      <c r="U10" s="11">
+        <v>8353078.9401600007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>18715000</v>
+      </c>
+      <c r="B11" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="11">
+        <v>-825</v>
+      </c>
+      <c r="F11" s="11">
+        <v>108665</v>
+      </c>
+      <c r="G11" s="11">
+        <v>17434.000000000004</v>
+      </c>
+      <c r="H11" s="11">
+        <v>19751.678240000001</v>
+      </c>
+      <c r="I11" s="11">
+        <v>72518.999999999985</v>
+      </c>
+      <c r="J11" s="11">
+        <v>1824.9999999999995</v>
+      </c>
+      <c r="K11" s="11">
+        <v>6519507.7608800009</v>
+      </c>
+      <c r="L11" s="11">
+        <v>26.6</v>
+      </c>
+      <c r="M11" s="11">
+        <v>270.99999999999818</v>
+      </c>
+      <c r="N11" s="11">
+        <v>292.99999999999886</v>
+      </c>
+      <c r="O11" s="11">
+        <v>225.39999999999932</v>
+      </c>
+      <c r="P11" s="11">
+        <v>2036.9999999998449</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>25366.999999999985</v>
+      </c>
+      <c r="R11" s="11">
+        <v>245884.47409999909</v>
+      </c>
+      <c r="S11" s="11">
+        <v>33.999999999999908</v>
+      </c>
+      <c r="T11" s="11">
+        <v>5712.9999999999991</v>
+      </c>
+      <c r="U11" s="11">
+        <v>12403303.24303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>1606000</v>
+      </c>
+      <c r="B12" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="11">
+        <v>2</v>
+      </c>
+      <c r="E12" s="11">
+        <v>-168</v>
+      </c>
+      <c r="F12" s="11">
+        <v>9622.9999999999964</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1207.9999999999993</v>
+      </c>
+      <c r="H12" s="11">
+        <v>16635.344249999991</v>
+      </c>
+      <c r="I12" s="11">
+        <v>3746.5999999999967</v>
+      </c>
+      <c r="J12" s="11">
+        <v>44.99999999999995</v>
+      </c>
+      <c r="K12" s="11">
+        <v>79286.091859999928</v>
+      </c>
+      <c r="L12" s="11">
+        <v>30.1</v>
+      </c>
+      <c r="M12" s="11">
+        <v>32.999999999999773</v>
+      </c>
+      <c r="N12" s="11">
+        <v>9.9999999999999485</v>
+      </c>
+      <c r="O12" s="11">
+        <v>212.39999999999975</v>
+      </c>
+      <c r="P12" s="11">
+        <v>22989.999999999982</v>
+      </c>
+      <c r="Q12" s="11">
+        <v>7487.889999999994</v>
+      </c>
+      <c r="R12" s="11">
+        <v>613356.16829999944</v>
+      </c>
+      <c r="S12" s="11">
+        <v>14.999999999999956</v>
+      </c>
+      <c r="T12" s="11">
+        <v>672.99999999999989</v>
+      </c>
+      <c r="U12" s="11">
+        <v>232900.09079999954</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>1620000</v>
+      </c>
+      <c r="B13" s="11">
+        <v>2018</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="11">
+        <v>2</v>
+      </c>
+      <c r="E13" s="11">
+        <v>-174</v>
+      </c>
+      <c r="F13" s="11">
+        <v>16685</v>
+      </c>
+      <c r="G13" s="11">
+        <v>2386</v>
+      </c>
+      <c r="H13" s="11">
+        <v>16273.3732</v>
+      </c>
+      <c r="I13" s="11">
+        <v>10592.199999999999</v>
+      </c>
+      <c r="J13" s="11">
+        <v>377.99999999999972</v>
+      </c>
+      <c r="K13" s="11">
+        <v>398404.10683999996</v>
+      </c>
+      <c r="L13" s="11">
+        <v>26.4</v>
+      </c>
+      <c r="M13" s="11">
+        <v>27.999999999999833</v>
+      </c>
+      <c r="N13" s="11">
+        <v>22.999999999999915</v>
+      </c>
+      <c r="O13" s="11">
+        <v>800.99999999999955</v>
+      </c>
+      <c r="P13" s="11">
+        <v>112136.99999999997</v>
+      </c>
+      <c r="Q13" s="11">
+        <v>9244.5999999999931</v>
+      </c>
+      <c r="R13" s="11">
+        <v>1610842.1835999999</v>
+      </c>
+      <c r="S13" s="11">
+        <v>21.999999999999957</v>
+      </c>
+      <c r="T13" s="11">
+        <v>624.00000000000011</v>
+      </c>
+      <c r="U13" s="11">
+        <v>1492496.0792400001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>1719000</v>
+      </c>
+      <c r="B14" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="11">
+        <v>2</v>
+      </c>
+      <c r="E14" s="11">
+        <v>-193</v>
+      </c>
+      <c r="F14" s="11">
+        <v>40956</v>
+      </c>
+      <c r="G14" s="11">
+        <v>6906.9999999999973</v>
+      </c>
+      <c r="H14" s="11">
+        <v>16179.493109999999</v>
+      </c>
+      <c r="I14" s="11">
+        <v>45679.399999999994</v>
+      </c>
+      <c r="J14" s="11">
+        <v>943.99999999999955</v>
+      </c>
+      <c r="K14" s="11">
+        <v>1135992.2059199996</v>
+      </c>
+      <c r="L14" s="11">
+        <v>22.9</v>
+      </c>
+      <c r="M14" s="11">
+        <v>86.999999999999389</v>
+      </c>
+      <c r="N14" s="11">
+        <v>196.9999999999992</v>
+      </c>
+      <c r="O14" s="11">
+        <v>2450.9999999999986</v>
+      </c>
+      <c r="P14" s="11">
+        <v>49269.999999999935</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>10475.609999999997</v>
+      </c>
+      <c r="R14" s="11">
+        <v>832899.14939999871</v>
+      </c>
+      <c r="S14" s="11">
+        <v>26.99999999999994</v>
+      </c>
+      <c r="T14" s="11">
+        <v>1959.9999999999998</v>
+      </c>
+      <c r="U14" s="11">
+        <v>1961160.027659998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>4621000</v>
+      </c>
+      <c r="B15" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="11">
+        <v>2</v>
+      </c>
+      <c r="E15" s="11">
+        <v>-121</v>
+      </c>
+      <c r="F15" s="11">
+        <v>24184.999999999989</v>
+      </c>
+      <c r="G15" s="11">
+        <v>4568.9999999999982</v>
+      </c>
+      <c r="H15" s="11">
+        <v>21418.87329</v>
+      </c>
+      <c r="I15" s="11">
+        <v>4933.5999999999949</v>
+      </c>
+      <c r="J15" s="11">
+        <v>130.99999999999977</v>
+      </c>
+      <c r="K15" s="11">
+        <v>143687.26248999985</v>
+      </c>
+      <c r="L15" s="11">
+        <v>22.3</v>
+      </c>
+      <c r="M15" s="11">
+        <v>103.9999999999993</v>
+      </c>
+      <c r="N15" s="11">
+        <v>2.9999999999999765</v>
+      </c>
+      <c r="O15" s="11">
+        <v>316.99999999999955</v>
+      </c>
+      <c r="P15" s="11">
+        <v>106497.99999999996</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>19137.909999999989</v>
+      </c>
+      <c r="R15" s="11">
+        <v>3427876.6054999977</v>
+      </c>
+      <c r="S15" s="11">
+        <v>50.999999999999886</v>
+      </c>
+      <c r="T15" s="11">
+        <v>1217.9999999999995</v>
+      </c>
+      <c r="U15" s="11">
+        <v>3524494.8488999987</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>36616000</v>
+      </c>
+      <c r="B16" s="11">
+        <v>2017</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="11">
+        <v>2</v>
+      </c>
+      <c r="E16" s="11">
+        <v>-158</v>
+      </c>
+      <c r="F16" s="11">
+        <v>12565.999999999991</v>
+      </c>
+      <c r="G16" s="11">
+        <v>2093.9999999999991</v>
+      </c>
+      <c r="H16" s="11">
+        <v>16955.84604</v>
+      </c>
+      <c r="I16" s="11">
+        <v>7192.4999999999927</v>
+      </c>
+      <c r="J16" s="11">
+        <v>449.99999999999943</v>
+      </c>
+      <c r="K16" s="11">
+        <v>298227.95619999972</v>
+      </c>
+      <c r="L16" s="11">
+        <v>30.03</v>
+      </c>
+      <c r="M16" s="11">
+        <v>59.999999999999581</v>
+      </c>
+      <c r="N16" s="11">
+        <v>14.999999999999922</v>
+      </c>
+      <c r="O16" s="11">
+        <v>647.79999999999916</v>
+      </c>
+      <c r="P16" s="11">
+        <v>25719.999999999982</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>20804.14999999998</v>
+      </c>
+      <c r="R16" s="11">
+        <v>1533618.0888999989</v>
+      </c>
+      <c r="S16" s="11">
+        <v>21.999999999999932</v>
+      </c>
+      <c r="T16" s="11">
+        <v>676.99999999999955</v>
+      </c>
+      <c r="U16" s="11">
+        <v>1868542.2159599983</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>1641000</v>
+      </c>
+      <c r="B17" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="11">
+        <v>3</v>
+      </c>
+      <c r="E17" s="11">
+        <v>-76</v>
+      </c>
+      <c r="F17" s="11">
+        <v>4183.9999999999918</v>
+      </c>
+      <c r="G17" s="11">
+        <v>788.99999999999841</v>
+      </c>
+      <c r="H17" s="11">
+        <v>19068.8688</v>
+      </c>
+      <c r="I17" s="11">
+        <v>1820.9999999999964</v>
+      </c>
+      <c r="J17" s="11">
+        <v>79.999999999999787</v>
+      </c>
+      <c r="K17" s="11">
+        <v>57968.611199999868</v>
+      </c>
+      <c r="L17" s="11">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="M17" s="11">
+        <v>12.999999999999892</v>
+      </c>
+      <c r="N17" s="11">
+        <v>1.9999999999999847</v>
+      </c>
+      <c r="O17" s="11">
+        <v>81.399999999999764</v>
+      </c>
+      <c r="P17" s="11">
+        <v>32010.999999999935</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>1244.4599999999969</v>
+      </c>
+      <c r="R17" s="11">
+        <v>838591.639199998</v>
+      </c>
+      <c r="S17" s="11">
+        <v>9.9999999999999591</v>
+      </c>
+      <c r="T17" s="11">
+        <v>251.99999999999952</v>
+      </c>
+      <c r="U17" s="11">
+        <v>750105.80711999815</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>3630000</v>
+      </c>
+      <c r="B18" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="11">
+        <v>3</v>
+      </c>
+      <c r="E18" s="11">
+        <v>-953</v>
+      </c>
+      <c r="F18" s="11">
+        <v>95828.000000000015</v>
+      </c>
+      <c r="G18" s="11">
+        <v>13438.999999999998</v>
+      </c>
+      <c r="H18" s="11">
+        <v>21170.54232</v>
+      </c>
+      <c r="I18" s="11">
+        <v>70891.10000000002</v>
+      </c>
+      <c r="J18" s="11">
+        <v>2106.9999999999986</v>
+      </c>
+      <c r="K18" s="11">
+        <v>2932758.8092799997</v>
+      </c>
+      <c r="L18" s="11">
+        <v>27.2</v>
+      </c>
+      <c r="M18" s="11">
+        <v>193.99999999999883</v>
+      </c>
+      <c r="N18" s="11">
+        <v>221.99999999999912</v>
+      </c>
+      <c r="O18" s="11">
+        <v>793.09999999999945</v>
+      </c>
+      <c r="P18" s="11">
+        <v>1149829.0000000002</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>72866.099999999977</v>
+      </c>
+      <c r="R18" s="11">
+        <v>9782808.4583999943</v>
+      </c>
+      <c r="S18" s="11">
+        <v>26.999999999999911</v>
+      </c>
+      <c r="T18" s="11">
+        <v>3887.9999999999995</v>
+      </c>
+      <c r="U18" s="11">
+        <v>9535558.9931999948</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>18652000</v>
+      </c>
+      <c r="B19" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="11">
+        <v>3</v>
+      </c>
+      <c r="E19" s="11">
+        <v>-188</v>
+      </c>
+      <c r="F19" s="11">
+        <v>17569.999999999989</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1887.9999999999989</v>
+      </c>
+      <c r="H19" s="11">
+        <v>18376.923200000001</v>
+      </c>
+      <c r="I19" s="11">
+        <v>8486.1999999999953</v>
+      </c>
+      <c r="J19" s="11">
+        <v>234.99999999999972</v>
+      </c>
+      <c r="K19" s="11">
+        <v>341592.53969999967</v>
+      </c>
+      <c r="L19" s="11">
+        <v>26.3</v>
+      </c>
+      <c r="M19" s="11">
+        <v>155.99999999999895</v>
+      </c>
+      <c r="N19" s="11">
+        <v>56.999999999999723</v>
+      </c>
+      <c r="O19" s="11">
+        <v>389.39999999999952</v>
+      </c>
+      <c r="P19" s="11">
+        <v>182951.9999999998</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>19100.999999999978</v>
+      </c>
+      <c r="R19" s="11">
+        <v>2366184.0724999984</v>
+      </c>
+      <c r="S19" s="11">
+        <v>24.999999999999932</v>
+      </c>
+      <c r="T19" s="11">
+        <v>790.99999999999943</v>
+      </c>
+      <c r="U19" s="11">
+        <v>322435.87408999965</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>22712000</v>
+      </c>
+      <c r="B20" s="11">
+        <v>2018</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="11">
+        <v>3</v>
+      </c>
+      <c r="E20" s="11">
+        <v>-483</v>
+      </c>
+      <c r="F20" s="11">
+        <v>120926</v>
+      </c>
+      <c r="G20" s="11">
+        <v>20037.999999999996</v>
+      </c>
+      <c r="H20" s="11">
+        <v>25152.816680000011</v>
+      </c>
+      <c r="I20" s="11">
+        <v>72911.599999999991</v>
+      </c>
+      <c r="J20" s="11">
+        <v>2549.9999999999977</v>
+      </c>
+      <c r="K20" s="11">
+        <v>4713511.9352799999</v>
+      </c>
+      <c r="L20" s="11">
+        <v>29.9</v>
+      </c>
+      <c r="M20" s="11">
+        <v>195.99999999999872</v>
+      </c>
+      <c r="N20" s="11">
+        <v>248.99999999999895</v>
+      </c>
+      <c r="O20" s="11">
+        <v>1123.1999999999985</v>
+      </c>
+      <c r="P20" s="11">
+        <v>1264806.9999999993</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>104307.92999999998</v>
+      </c>
+      <c r="R20" s="11">
+        <v>2214641.3434399972</v>
+      </c>
+      <c r="S20" s="11">
+        <v>34.999999999999915</v>
+      </c>
+      <c r="T20" s="11">
+        <v>6308.9999999999991</v>
+      </c>
+      <c r="U20" s="11">
+        <v>26988496.705479994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>53725000</v>
+      </c>
+      <c r="B21" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="11">
+        <v>3</v>
+      </c>
+      <c r="E21" s="11">
+        <v>-523</v>
+      </c>
+      <c r="F21" s="11">
+        <v>50473.999999999993</v>
+      </c>
+      <c r="G21" s="11">
+        <v>8680.9999999999982</v>
+      </c>
+      <c r="H21" s="11">
+        <v>19397.3076</v>
+      </c>
+      <c r="I21" s="11">
+        <v>32935.899999999994</v>
+      </c>
+      <c r="J21" s="11">
+        <v>1673.9999999999982</v>
+      </c>
+      <c r="K21" s="11">
+        <v>1330729.4930399999</v>
+      </c>
+      <c r="L21" s="11">
+        <v>25.1</v>
+      </c>
+      <c r="M21" s="11">
+        <v>158.99999999999895</v>
+      </c>
+      <c r="N21" s="11">
+        <v>184.99999999999918</v>
+      </c>
+      <c r="O21" s="11">
+        <v>386.19999999999953</v>
+      </c>
+      <c r="P21" s="11">
+        <v>810919.99999999977</v>
+      </c>
+      <c r="Q21" s="11">
+        <v>182696</v>
+      </c>
+      <c r="R21" s="11">
+        <v>5519372.8535999991</v>
+      </c>
+      <c r="S21" s="11">
+        <v>38.999999999999908</v>
+      </c>
+      <c r="T21" s="11">
+        <v>2499.9999999999995</v>
+      </c>
+      <c r="U21" s="11">
+        <v>3749387.5015199976</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>1706000</v>
+      </c>
+      <c r="B22" s="11">
+        <v>2014</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="11">
+        <v>4</v>
+      </c>
+      <c r="E22" s="11">
+        <v>-199</v>
+      </c>
+      <c r="F22" s="11">
+        <v>47578.999999999993</v>
+      </c>
+      <c r="G22" s="11">
+        <v>11633.999999999998</v>
+      </c>
+      <c r="H22" s="11">
+        <v>24954.799999999999</v>
+      </c>
+      <c r="I22" s="11">
+        <v>37654.999999999985</v>
+      </c>
+      <c r="J22" s="11">
+        <v>898.99999999999943</v>
+      </c>
+      <c r="K22" s="11">
+        <v>1350652</v>
+      </c>
+      <c r="L22" s="11">
+        <v>23.5</v>
+      </c>
+      <c r="M22" s="11">
+        <v>69.999999999999503</v>
+      </c>
+      <c r="N22" s="11">
+        <v>171.99999999999929</v>
+      </c>
+      <c r="O22" s="11">
+        <v>201.0999999999998</v>
+      </c>
+      <c r="P22" s="11">
+        <v>14598.999999999955</v>
+      </c>
+      <c r="Q22" s="11">
+        <v>16640.329999999991</v>
+      </c>
+      <c r="R22" s="11">
+        <v>232538.99999999936</v>
+      </c>
+      <c r="S22" s="11">
+        <v>10.999999999999968</v>
+      </c>
+      <c r="T22" s="11">
+        <v>2737.9999999999991</v>
+      </c>
+      <c r="U22" s="11">
+        <v>32418265.199999992</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>5634000</v>
+      </c>
+      <c r="B23" s="11">
+        <v>2017</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="11">
+        <v>4</v>
+      </c>
+      <c r="E23" s="11">
+        <v>-310</v>
+      </c>
+      <c r="F23" s="11">
+        <v>28553</v>
+      </c>
+      <c r="G23" s="11">
+        <v>6935.9999999999991</v>
+      </c>
+      <c r="H23" s="11">
+        <v>34591.617420000002</v>
+      </c>
+      <c r="I23" s="11">
+        <v>13338.599999999997</v>
+      </c>
+      <c r="J23" s="11">
+        <v>494.99999999999943</v>
+      </c>
+      <c r="K23" s="11">
+        <v>139069.51849999998</v>
+      </c>
+      <c r="L23" s="11">
+        <v>22.9</v>
+      </c>
+      <c r="M23" s="11">
+        <v>76.999999999999531</v>
+      </c>
+      <c r="N23" s="11">
+        <v>124.99999999999952</v>
+      </c>
+      <c r="O23" s="11">
+        <v>169.2999999999999</v>
+      </c>
+      <c r="P23" s="11">
+        <v>19625.999999999978</v>
+      </c>
+      <c r="Q23" s="11">
+        <v>10308.619999999997</v>
+      </c>
+      <c r="R23" s="11">
+        <v>429026.07919999963</v>
+      </c>
+      <c r="S23" s="11">
+        <v>11.999999999999972</v>
+      </c>
+      <c r="T23" s="11">
+        <v>2062</v>
+      </c>
+      <c r="U23" s="11">
+        <v>13315114.298400002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>25738000</v>
+      </c>
+      <c r="B24" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="11">
+        <v>4</v>
+      </c>
+      <c r="E24" s="11">
+        <v>-236</v>
+      </c>
+      <c r="F24" s="11">
+        <v>79746</v>
+      </c>
+      <c r="G24" s="11">
+        <v>16843</v>
+      </c>
+      <c r="H24" s="11">
+        <v>35339.908029999999</v>
+      </c>
+      <c r="I24" s="11">
+        <v>73491.599999999991</v>
+      </c>
+      <c r="J24" s="11">
+        <v>2645.9999999999991</v>
+      </c>
+      <c r="K24" s="11">
+        <v>2006637.54357</v>
+      </c>
+      <c r="L24" s="11">
+        <v>24.6</v>
+      </c>
+      <c r="M24" s="11">
+        <v>164.99999999999895</v>
+      </c>
+      <c r="N24" s="11">
+        <v>232.99999999999903</v>
+      </c>
+      <c r="O24" s="11">
+        <v>188.49999999999935</v>
+      </c>
+      <c r="P24" s="11">
+        <v>1592.9999999998829</v>
+      </c>
+      <c r="Q24" s="11">
+        <v>23405.999999999971</v>
+      </c>
+      <c r="R24" s="11">
+        <v>313421.54109999974</v>
+      </c>
+      <c r="S24" s="11">
+        <v>7.9999999999999671</v>
+      </c>
+      <c r="T24" s="11">
+        <v>5536</v>
+      </c>
+      <c r="U24" s="11">
+        <v>37484508.028549999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>36704000</v>
+      </c>
+      <c r="B25" s="11">
+        <v>2018</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="11">
+        <v>4</v>
+      </c>
+      <c r="E25" s="11">
+        <v>-472</v>
+      </c>
+      <c r="F25" s="11">
+        <v>57687</v>
+      </c>
+      <c r="G25" s="11">
+        <v>11292</v>
+      </c>
+      <c r="H25" s="11">
+        <v>23845.612519999999</v>
+      </c>
+      <c r="I25" s="11">
+        <v>33352.599999999984</v>
+      </c>
+      <c r="J25" s="11">
+        <v>1263.9999999999993</v>
+      </c>
+      <c r="K25" s="11">
+        <v>1716389.6294400003</v>
+      </c>
+      <c r="L25" s="11">
+        <v>29.41</v>
+      </c>
+      <c r="M25" s="11">
+        <v>70.999999999999531</v>
+      </c>
+      <c r="N25" s="11">
+        <v>230.99999999999903</v>
+      </c>
+      <c r="O25" s="11">
+        <v>233.29999999999964</v>
+      </c>
+      <c r="P25" s="11">
+        <v>383.99999999993003</v>
+      </c>
+      <c r="Q25" s="11">
+        <v>37867.999999999993</v>
+      </c>
+      <c r="R25" s="11">
+        <v>322803.30879999872</v>
+      </c>
+      <c r="S25" s="11">
+        <v>0.99999999999999423</v>
+      </c>
+      <c r="T25" s="11">
+        <v>2426.9999999999995</v>
+      </c>
+      <c r="U25" s="11">
+        <v>32139963.465120006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>65753000</v>
+      </c>
+      <c r="B26" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="11">
+        <v>4</v>
+      </c>
+      <c r="E26" s="11">
+        <v>-402</v>
+      </c>
+      <c r="F26" s="11">
+        <v>141368</v>
+      </c>
+      <c r="G26" s="11">
+        <v>33537</v>
+      </c>
+      <c r="H26" s="11">
+        <v>27126.22694</v>
+      </c>
+      <c r="I26" s="11">
+        <v>58200</v>
+      </c>
+      <c r="J26" s="11">
+        <v>2876.9999999999973</v>
+      </c>
+      <c r="K26" s="11">
+        <v>10541809.012150001</v>
+      </c>
+      <c r="L26" s="11">
+        <v>31.4</v>
+      </c>
+      <c r="M26" s="11">
+        <v>306.99999999999795</v>
+      </c>
+      <c r="N26" s="11">
+        <v>198.99999999999918</v>
+      </c>
+      <c r="O26" s="11">
+        <v>474.69999999999879</v>
+      </c>
+      <c r="P26" s="11">
+        <v>595570.99999999977</v>
+      </c>
+      <c r="Q26" s="11">
+        <v>59771.349999999991</v>
+      </c>
+      <c r="R26" s="11">
+        <v>1632754.1328999992</v>
+      </c>
+      <c r="S26" s="11">
+        <v>90.999999999999801</v>
+      </c>
+      <c r="T26" s="11">
+        <v>9371</v>
+      </c>
+      <c r="U26" s="11">
+        <v>79424596.731749997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>1625000</v>
+      </c>
+      <c r="B27" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="11">
+        <v>5</v>
+      </c>
+      <c r="E27" s="11">
+        <v>-294</v>
+      </c>
+      <c r="F27" s="11">
+        <v>23671.999999999989</v>
+      </c>
+      <c r="G27" s="11">
+        <v>2819.9999999999991</v>
+      </c>
+      <c r="H27" s="11">
+        <v>17545.93204</v>
+      </c>
+      <c r="I27" s="11">
+        <v>16399.19999999999</v>
+      </c>
+      <c r="J27" s="11">
+        <v>346.9999999999996</v>
+      </c>
+      <c r="K27" s="11">
+        <v>573514.04293999961</v>
+      </c>
+      <c r="L27" s="11">
+        <v>28</v>
+      </c>
+      <c r="M27" s="11">
+        <v>64.999999999999574</v>
+      </c>
+      <c r="N27" s="11">
+        <v>59.999999999999716</v>
+      </c>
+      <c r="O27" s="11">
+        <v>382.49999999999949</v>
+      </c>
+      <c r="P27" s="11">
+        <v>39639.999999999935</v>
+      </c>
+      <c r="Q27" s="11">
+        <v>9314.3999999999924</v>
+      </c>
+      <c r="R27" s="11">
+        <v>3234408.7671999987</v>
+      </c>
+      <c r="S27" s="11">
+        <v>17.99999999999995</v>
+      </c>
+      <c r="T27" s="11">
+        <v>744.99999999999955</v>
+      </c>
+      <c r="U27" s="11">
+        <v>828015.21829999832</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>3654000</v>
+      </c>
+      <c r="B28" s="11">
+        <v>2019</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="11">
+        <v>5</v>
+      </c>
+      <c r="E28" s="11">
+        <v>-541</v>
+      </c>
+      <c r="F28" s="11">
+        <v>116468</v>
+      </c>
+      <c r="G28" s="11">
+        <v>21239.000000000004</v>
+      </c>
+      <c r="H28" s="11">
+        <v>23604.910929999998</v>
+      </c>
+      <c r="I28" s="11">
+        <v>64664.399999999987</v>
+      </c>
+      <c r="J28" s="11">
+        <v>2076.9999999999995</v>
+      </c>
+      <c r="K28" s="11">
+        <v>4676977.1911799992</v>
+      </c>
+      <c r="L28" s="11">
+        <v>30.2</v>
+      </c>
+      <c r="M28" s="11">
+        <v>300.99999999999807</v>
+      </c>
+      <c r="N28" s="11">
+        <v>303.99999999999869</v>
+      </c>
+      <c r="O28" s="11">
+        <v>783.79999999999882</v>
+      </c>
+      <c r="P28" s="11">
+        <v>202571.00000000003</v>
+      </c>
+      <c r="Q28" s="11">
+        <v>87368.909999999974</v>
+      </c>
+      <c r="R28" s="11">
+        <v>8408723.8795999978</v>
+      </c>
+      <c r="S28" s="11">
+        <v>34.999999999999901</v>
+      </c>
+      <c r="T28" s="11">
+        <v>4502</v>
+      </c>
+      <c r="U28" s="11">
+        <v>19397519.885310002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>4722000</v>
+      </c>
+      <c r="B29" s="11">
+        <v>2015</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="11">
+        <v>5</v>
+      </c>
+      <c r="E29" s="11">
+        <v>-192</v>
+      </c>
+      <c r="F29" s="11">
+        <v>64841.999999999993</v>
+      </c>
+      <c r="G29" s="11">
+        <v>15028.999999999996</v>
+      </c>
+      <c r="H29" s="11">
+        <v>25869.387780000001</v>
+      </c>
+      <c r="I29" s="11">
+        <v>17235.499999999989</v>
+      </c>
+      <c r="J29" s="11">
+        <v>1123.9999999999986</v>
+      </c>
+      <c r="K29" s="11">
+        <v>866008.93850999954</v>
+      </c>
+      <c r="L29" s="11">
+        <v>23.8</v>
+      </c>
+      <c r="M29" s="11">
+        <v>124.99999999999919</v>
+      </c>
+      <c r="N29" s="11">
+        <v>194.99999999999915</v>
+      </c>
+      <c r="O29" s="11">
+        <v>235.39999999999975</v>
+      </c>
+      <c r="P29" s="11">
+        <v>2168.999999999995</v>
+      </c>
+      <c r="Q29" s="11">
+        <v>22439.059999999987</v>
+      </c>
+      <c r="R29" s="11">
+        <v>259751.15039999882</v>
+      </c>
+      <c r="S29" s="11">
+        <v>11.999999999999948</v>
+      </c>
+      <c r="T29" s="11">
+        <v>3210.9999999999995</v>
+      </c>
+      <c r="U29" s="11">
+        <v>9430951.7147999946</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>7726000</v>
+      </c>
+      <c r="B30" s="11">
+        <v>2020</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="11">
+        <v>5</v>
+      </c>
+      <c r="E30" s="11">
+        <v>-300</v>
+      </c>
+      <c r="F30" s="11">
+        <v>64100</v>
+      </c>
+      <c r="G30" s="11">
+        <v>9192</v>
+      </c>
+      <c r="H30" s="11">
+        <v>21205.026720000002</v>
+      </c>
+      <c r="I30" s="11">
+        <v>59994</v>
+      </c>
+      <c r="J30" s="11">
+        <v>1042.9999999999993</v>
+      </c>
+      <c r="K30" s="11">
+        <v>1194600.3487199994</v>
+      </c>
+      <c r="L30" s="11">
+        <v>24.81</v>
+      </c>
+      <c r="M30" s="11">
+        <v>140.99999999999912</v>
+      </c>
+      <c r="N30" s="11">
+        <v>92.999999999999559</v>
+      </c>
+      <c r="O30" s="11">
+        <v>563.59999999999923</v>
+      </c>
+      <c r="P30" s="11">
+        <v>35895.999999999993</v>
+      </c>
+      <c r="Q30" s="11">
+        <v>57654.419999999991</v>
+      </c>
+      <c r="R30" s="11">
+        <v>8271274.1760000018</v>
+      </c>
+      <c r="S30" s="11">
+        <v>36.999999999999908</v>
+      </c>
+      <c r="T30" s="11">
+        <v>3089.9999999999995</v>
+      </c>
+      <c r="U30" s="11">
+        <v>7029925.2345599988</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>60730000</v>
+      </c>
+      <c r="B31" s="11">
+        <v>2021</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="11">
+        <v>5</v>
+      </c>
+      <c r="E31" s="11">
+        <v>-429</v>
+      </c>
+      <c r="F31" s="11">
+        <v>105038</v>
+      </c>
+      <c r="G31" s="11">
+        <v>11442</v>
+      </c>
+      <c r="H31" s="11">
+        <v>18218.315640000001</v>
+      </c>
+      <c r="I31" s="11">
+        <v>69421.599999999991</v>
+      </c>
+      <c r="J31" s="11">
+        <v>79.999999999999517</v>
+      </c>
+      <c r="K31" s="11">
+        <v>3389505.0557000008</v>
+      </c>
+      <c r="L31" s="11">
+        <v>21.85</v>
+      </c>
+      <c r="M31" s="11">
+        <v>164.99999999999895</v>
+      </c>
+      <c r="N31" s="11">
+        <v>248.99999999999898</v>
+      </c>
+      <c r="O31" s="11">
+        <v>369.09999999999923</v>
+      </c>
+      <c r="P31" s="11">
+        <v>18256.999999999818</v>
+      </c>
+      <c r="Q31" s="11">
+        <v>57789.999999999949</v>
+      </c>
+      <c r="R31" s="11">
+        <v>521260.11459999764</v>
+      </c>
+      <c r="S31" s="11">
+        <v>5.9999999999999627</v>
+      </c>
+      <c r="T31" s="11">
+        <v>3403</v>
+      </c>
+      <c r="U31" s="11">
+        <v>5939939.1027599983</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>